<commit_message>
MAPEI order ,work in progress
git-tfs-id: [https://gyorgyiantal.visualstudio.com]$/PMap/PMap;C869
</commit_message>
<xml_diff>
--- a/doc/Mapei/NetMover adatexport.xlsx
+++ b/doc/Mapei/NetMover adatexport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerenyia\OneDrive - Mapei Group\Mapei\WIP\projektek\2018 Q2 Netmover planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\source\PMap\doc\Mapei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{318D0117-6FD3-4B75-9D35-FC51FBD13CA9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C84FCDF8-9E37-43D1-8AFF-160BE84B291D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Y$2:$AA$1002</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2100,7 +2099,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2161,7 +2160,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2472,12 +2471,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15089BF-ECEC-44CB-8868-57C63A21BB0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2488,7 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
@@ -79726,7 +79725,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="Y2:AA1002" xr:uid="{1A64F983-2E2E-4FB9-BACC-55379B9BA88E}"/>
+  <autoFilter ref="Y2:AA1002"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>